<commit_message>
Fixed edge source pin alignement
</commit_message>
<xml_diff>
--- a/examples/OpenFPGA_basic/baseline_l4/switchbox_main.xlsx
+++ b/examples/OpenFPGA_basic/baseline_l4/switchbox_main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="72">
   <si>
     <t>Left</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>OPIN</t>
@@ -323,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +366,12 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -689,69 +698,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="62" max="62" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="63" max="63" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="16" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="18" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="50" max="50" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="51" max="51" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="52" max="52" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="53" max="53" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="54" max="54" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="55" max="55" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="56" max="56" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="57" max="57" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="58" max="58" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="59" max="59" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="60" max="60" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="61" max="61" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="62" max="62" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="63" max="63" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -2337,7 +2346,9 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="13"/>
+      <c r="L18" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -2408,7 +2419,9 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="13"/>
+      <c r="L19" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -2479,7 +2492,9 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="13"/>
+      <c r="L20" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -2550,7 +2565,9 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="13"/>
+      <c r="L21" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -3481,7 +3498,9 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
+      <c r="L34" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
@@ -3552,7 +3571,9 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
+      <c r="L35" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
@@ -3623,7 +3644,9 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
+      <c r="L36" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -3694,7 +3717,9 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
+      <c r="L37" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
       <c r="O37" s="13"/>
@@ -4561,7 +4586,9 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="13"/>
-      <c r="M49" s="5"/>
+      <c r="M49" s="15" t="s">
+        <v>50</v>
+      </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
@@ -4633,8 +4660,12 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="5"/>
+      <c r="L50" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M50" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
@@ -4704,8 +4735,12 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="5"/>
+      <c r="L51" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M51" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
@@ -4775,8 +4810,12 @@
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="5"/>
+      <c r="L52" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M52" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
@@ -4846,8 +4885,12 @@
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
+      <c r="L53" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M53" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
@@ -5785,7 +5828,9 @@
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
-      <c r="L66" s="13"/>
+      <c r="L66" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -5856,7 +5901,9 @@
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
-      <c r="L67" s="13"/>
+      <c r="L67" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -5927,7 +5974,9 @@
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
-      <c r="L68" s="13"/>
+      <c r="L68" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="M68" s="5"/>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
@@ -5998,7 +6047,9 @@
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
+      <c r="L69" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="M69" s="5"/>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -6053,14 +6104,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="4">
         <v>47</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -6124,14 +6175,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="4">
         <v>48</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
@@ -6195,14 +6246,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="4">
         <v>49</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E72" s="13"/>
       <c r="F72" s="13"/>
@@ -6266,14 +6317,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="4">
         <v>50</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
@@ -6337,14 +6388,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="4">
         <v>51</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
@@ -6408,14 +6459,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="4">
         <v>52</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
@@ -6479,14 +6530,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="4">
         <v>53</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E76" s="13"/>
       <c r="F76" s="13"/>
@@ -6550,14 +6601,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="4">
         <v>54</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
@@ -6621,14 +6672,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="4">
         <v>55</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
@@ -6692,14 +6743,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="4">
         <v>56</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
@@ -6763,14 +6814,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="4">
         <v>57</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E80" s="13"/>
       <c r="F80" s="13"/>
@@ -6834,14 +6885,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="4">
         <v>58</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E81" s="13"/>
       <c r="F81" s="13"/>
@@ -6905,14 +6956,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="4">
         <v>59</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
@@ -6976,14 +7027,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="4">
         <v>60</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E83" s="13"/>
       <c r="F83" s="13"/>
@@ -7047,14 +7098,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="4">
         <v>61</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
@@ -7118,14 +7169,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="4">
         <v>62</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E85" s="13"/>
       <c r="F85" s="13"/>
@@ -7189,14 +7240,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="4">
         <v>63</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -7260,14 +7311,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="4">
         <v>64</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E87" s="13"/>
       <c r="F87" s="13"/>
@@ -7331,14 +7382,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="4">
         <v>65</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E88" s="13"/>
       <c r="F88" s="13"/>
@@ -7402,14 +7453,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="4">
         <v>66</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>

</xml_diff>

<commit_message>
Added IPIN OPIN connections
</commit_message>
<xml_diff>
--- a/examples/OpenFPGA_basic/baseline_l4/switchbox_main.xlsx
+++ b/examples/OpenFPGA_basic/baseline_l4/switchbox_main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="71">
   <si>
     <t>Left</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>OPIN</t>
@@ -326,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,12 +363,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,69 +689,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="16" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="17" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="18" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="18" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="19" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="62" max="62" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="63" max="63" style="20" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="17" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="50" max="50" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="51" max="51" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="52" max="52" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="53" max="53" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="54" max="54" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="55" max="55" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="56" max="56" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="57" max="57" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="58" max="58" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="59" max="59" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="60" max="60" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="61" max="61" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="62" max="62" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="63" max="63" style="18" width="8.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -917,181 +908,181 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="6">
-        <f>countif(E4:E747, "=x")</f>
+        <f>COUNTIF(E4:E747, "=x")</f>
       </c>
       <c r="F3" s="6">
-        <f>countif(F4:F747, "=x")</f>
+        <f>COUNTIF(F4:F747, "=x")</f>
       </c>
       <c r="G3" s="6">
-        <f>countif(G4:G747, "=x")</f>
+        <f>COUNTIF(G4:G747, "=x")</f>
       </c>
       <c r="H3" s="6">
-        <f>countif(H4:H747, "=x")</f>
+        <f>COUNTIF(H4:H747, "=x")</f>
       </c>
       <c r="I3" s="7">
-        <f>countif(I4:I747, "=x")</f>
+        <f>COUNTIF(I4:I747, "=x")</f>
       </c>
       <c r="J3" s="7">
-        <f>countif(J4:J747, "=x")</f>
+        <f>COUNTIF(J4:J747, "=x")</f>
       </c>
       <c r="K3" s="7">
-        <f>countif(K4:K747, "=x")</f>
+        <f>COUNTIF(K4:K747, "=x")</f>
       </c>
       <c r="L3" s="7">
-        <f>countif(L4:L747, "=x")</f>
+        <f>COUNTIF(L4:L747, "=x")</f>
       </c>
       <c r="M3" s="8">
-        <f>countif(M4:M747, "=x")</f>
+        <f>COUNTIF(M4:M747, "=x")</f>
       </c>
       <c r="N3" s="8">
-        <f>countif(N4:N747, "=x")</f>
+        <f>COUNTIF(N4:N747, "=x")</f>
       </c>
       <c r="O3" s="8">
-        <f>countif(O4:O747, "=x")</f>
+        <f>COUNTIF(O4:O747, "=x")</f>
       </c>
       <c r="P3" s="8">
-        <f>countif(P4:P747, "=x")</f>
+        <f>COUNTIF(P4:P747, "=x")</f>
       </c>
       <c r="Q3" s="9">
-        <f>countif(Q4:Q747, "=x")</f>
+        <f>COUNTIF(Q4:Q747, "=x")</f>
       </c>
       <c r="R3" s="9">
-        <f>countif(R4:R747, "=x")</f>
+        <f>COUNTIF(R4:R747, "=x")</f>
       </c>
       <c r="S3" s="9">
-        <f>countif(S4:S747, "=x")</f>
+        <f>COUNTIF(S4:S747, "=x")</f>
       </c>
       <c r="T3" s="9">
-        <f>countif(T4:T747, "=x")</f>
+        <f>COUNTIF(T4:T747, "=x")</f>
       </c>
       <c r="U3" s="10">
-        <f>countif(U4:U747, "=x")</f>
+        <f>COUNTIF(U4:U747, "=x")</f>
       </c>
       <c r="V3" s="10">
-        <f>countif(V4:V747, "=x")</f>
+        <f>COUNTIF(V4:V747, "=x")</f>
       </c>
       <c r="W3" s="10">
-        <f>countif(W4:W747, "=x")</f>
+        <f>COUNTIF(W4:W747, "=x")</f>
       </c>
       <c r="X3" s="10">
-        <f>countif(X4:X747, "=x")</f>
+        <f>COUNTIF(X4:X747, "=x")</f>
       </c>
       <c r="Y3" s="10">
-        <f>countif(Y4:Y747, "=x")</f>
+        <f>COUNTIF(Y4:Y747, "=x")</f>
       </c>
       <c r="Z3" s="10">
-        <f>countif(Z4:Z747, "=x")</f>
+        <f>COUNTIF(Z4:Z747, "=x")</f>
       </c>
       <c r="AA3" s="10">
-        <f>countif(AA4:AA747, "=x")</f>
+        <f>COUNTIF(AA4:AA747, "=x")</f>
       </c>
       <c r="AB3" s="10">
-        <f>countif(AB4:AB747, "=x")</f>
+        <f>COUNTIF(AB4:AB747, "=x")</f>
       </c>
       <c r="AC3" s="10">
-        <f>countif(AC4:AC747, "=x")</f>
+        <f>COUNTIF(AC4:AC747, "=x")</f>
       </c>
       <c r="AD3" s="10">
-        <f>countif(AD4:AD747, "=x")</f>
+        <f>COUNTIF(AD4:AD747, "=x")</f>
       </c>
       <c r="AE3" s="10">
-        <f>countif(AE4:AE747, "=x")</f>
+        <f>COUNTIF(AE4:AE747, "=x")</f>
       </c>
       <c r="AF3" s="10">
-        <f>countif(AF4:AF747, "=x")</f>
+        <f>COUNTIF(AF4:AF747, "=x")</f>
       </c>
       <c r="AG3" s="10">
-        <f>countif(AG4:AG747, "=x")</f>
+        <f>COUNTIF(AG4:AG747, "=x")</f>
       </c>
       <c r="AH3" s="10">
-        <f>countif(AH4:AH747, "=x")</f>
+        <f>COUNTIF(AH4:AH747, "=x")</f>
       </c>
       <c r="AI3" s="10">
-        <f>countif(AI4:AI747, "=x")</f>
+        <f>COUNTIF(AI4:AI747, "=x")</f>
       </c>
       <c r="AJ3" s="10">
-        <f>countif(AJ4:AJ747, "=x")</f>
+        <f>COUNTIF(AJ4:AJ747, "=x")</f>
       </c>
       <c r="AK3" s="10">
-        <f>countif(AK4:AK747, "=x")</f>
+        <f>COUNTIF(AK4:AK747, "=x")</f>
       </c>
       <c r="AL3" s="10">
-        <f>countif(AL4:AL747, "=x")</f>
+        <f>COUNTIF(AL4:AL747, "=x")</f>
       </c>
       <c r="AM3" s="10">
-        <f>countif(AM4:AM747, "=x")</f>
+        <f>COUNTIF(AM4:AM747, "=x")</f>
       </c>
       <c r="AN3" s="10">
-        <f>countif(AN4:AN747, "=x")</f>
+        <f>COUNTIF(AN4:AN747, "=x")</f>
       </c>
       <c r="AO3" s="10">
-        <f>countif(AO4:AO747, "=x")</f>
+        <f>COUNTIF(AO4:AO747, "=x")</f>
       </c>
       <c r="AP3" s="10">
-        <f>countif(AP4:AP747, "=x")</f>
+        <f>COUNTIF(AP4:AP747, "=x")</f>
       </c>
       <c r="AQ3" s="10">
-        <f>countif(AQ4:AQ747, "=x")</f>
+        <f>COUNTIF(AQ4:AQ747, "=x")</f>
       </c>
       <c r="AR3" s="10">
-        <f>countif(AR4:AR747, "=x")</f>
+        <f>COUNTIF(AR4:AR747, "=x")</f>
       </c>
       <c r="AS3" s="10">
-        <f>countif(AS4:AS747, "=x")</f>
+        <f>COUNTIF(AS4:AS747, "=x")</f>
       </c>
       <c r="AT3" s="10">
-        <f>countif(AT4:AT747, "=x")</f>
+        <f>COUNTIF(AT4:AT747, "=x")</f>
       </c>
       <c r="AU3" s="10">
-        <f>countif(AU4:AU747, "=x")</f>
+        <f>COUNTIF(AU4:AU747, "=x")</f>
       </c>
       <c r="AV3" s="10">
-        <f>countif(AV4:AV747, "=x")</f>
+        <f>COUNTIF(AV4:AV747, "=x")</f>
       </c>
       <c r="AW3" s="10">
-        <f>countif(AW4:AW747, "=x")</f>
+        <f>COUNTIF(AW4:AW747, "=x")</f>
       </c>
       <c r="AX3" s="10">
-        <f>countif(AX4:AX747, "=x")</f>
+        <f>COUNTIF(AX4:AX747, "=x")</f>
       </c>
       <c r="AY3" s="10">
-        <f>countif(AY4:AY747, "=x")</f>
+        <f>COUNTIF(AY4:AY747, "=x")</f>
       </c>
       <c r="AZ3" s="10">
-        <f>countif(AZ4:AZ747, "=x")</f>
+        <f>COUNTIF(AZ4:AZ747, "=x")</f>
       </c>
       <c r="BA3" s="10">
-        <f>countif(BA4:BA747, "=x")</f>
+        <f>COUNTIF(BA4:BA747, "=x")</f>
       </c>
       <c r="BB3" s="10">
-        <f>countif(BB4:BB747, "=x")</f>
+        <f>COUNTIF(BB4:BB747, "=x")</f>
       </c>
       <c r="BC3" s="10">
-        <f>countif(BC4:BC747, "=x")</f>
+        <f>COUNTIF(BC4:BC747, "=x")</f>
       </c>
       <c r="BD3" s="10">
-        <f>countif(BD4:BD747, "=x")</f>
+        <f>COUNTIF(BD4:BD747, "=x")</f>
       </c>
       <c r="BE3" s="10">
-        <f>countif(BE4:BE747, "=x")</f>
+        <f>COUNTIF(BE4:BE747, "=x")</f>
       </c>
       <c r="BF3" s="10">
-        <f>countif(BF4:BF747, "=x")</f>
+        <f>COUNTIF(BF4:BF747, "=x")</f>
       </c>
       <c r="BG3" s="10">
-        <f>countif(BG4:BG747, "=x")</f>
+        <f>COUNTIF(BG4:BG747, "=x")</f>
       </c>
       <c r="BH3" s="10">
-        <f>countif(BH4:BH747, "=x")</f>
+        <f>COUNTIF(BH4:BH747, "=x")</f>
       </c>
       <c r="BI3" s="10">
-        <f>countif(BI4:BI747, "=x")</f>
+        <f>COUNTIF(BI4:BI747, "=x")</f>
       </c>
       <c r="BJ3" s="10">
-        <f>countif(BJ4:BJ747, "=x")</f>
+        <f>COUNTIF(BJ4:BJ747, "=x")</f>
       </c>
       <c r="BK3" s="10">
-        <f>countif(BK4:BK747, "=x")</f>
+        <f>COUNTIF(BK4:BK747, "=x")</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -1148,133 +1139,133 @@
         <v>4</v>
       </c>
       <c r="U4" s="4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="V4" s="4">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="W4" s="4">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="X4" s="4">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="Y4" s="4">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="Z4" s="4">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="AA4" s="4">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="AB4" s="4">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="AC4" s="4">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="AD4" s="4">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="AE4" s="4">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="AF4" s="4">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="AG4" s="4">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="AH4" s="4">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="AI4" s="4">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="AJ4" s="4">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="AK4" s="4">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="AL4" s="4">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="AM4" s="4">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="AN4" s="4">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="AO4" s="4">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="AP4" s="4">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="AQ4" s="4">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="AR4" s="4">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="AS4" s="4">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="AT4" s="4">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="AU4" s="4">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="AV4" s="4">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="AW4" s="4">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="AX4" s="4">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="AY4" s="4">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="AZ4" s="4">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="BA4" s="4">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="BB4" s="4">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="BC4" s="4">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="BD4" s="4">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="BE4" s="4">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="BF4" s="4">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="BG4" s="4">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="BH4" s="4">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="BI4" s="4">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="BJ4" s="4">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="BK4" s="4">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -1477,9 +1468,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I6" s="13"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -1491,7 +1480,9 @@
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="13"/>
+      <c r="U6" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="V6" s="13"/>
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
@@ -1550,9 +1541,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I7" s="13"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1623,9 +1612,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I8" s="13"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1696,9 +1683,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I9" s="13"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -2346,9 +2331,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="L18" s="13"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -2419,9 +2402,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="L19" s="13"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -2492,9 +2473,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="L20" s="13"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -2565,9 +2544,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="L21" s="13"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -3498,9 +3475,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="L34" s="13"/>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
@@ -3571,9 +3546,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="L35" s="13"/>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
@@ -3644,9 +3617,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="L36" s="13"/>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -3717,9 +3688,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="L37" s="13"/>
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
       <c r="O37" s="13"/>
@@ -3789,9 +3758,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-      <c r="I38" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I38" s="13"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -3862,9 +3829,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
-      <c r="I39" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I39" s="13"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
@@ -3935,9 +3900,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
-      <c r="I40" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I40" s="13"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
@@ -4008,9 +3971,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
-      <c r="I41" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I41" s="13"/>
       <c r="J41" s="13"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -4586,9 +4547,7 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="13"/>
-      <c r="M49" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="M49" s="5"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
@@ -4660,12 +4619,8 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
-      <c r="L50" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M50" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
@@ -4735,12 +4690,8 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
-      <c r="L51" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M51" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
@@ -4810,12 +4761,8 @@
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
-      <c r="L52" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M52" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
@@ -4885,12 +4832,8 @@
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
-      <c r="L53" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M53" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
@@ -4959,9 +4902,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
-      <c r="I54" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I54" s="13"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
@@ -5032,9 +4973,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
-      <c r="I55" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I55" s="13"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -5105,9 +5044,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-      <c r="I56" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I56" s="13"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
@@ -5178,9 +5115,7 @@
       <c r="F57" s="13"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
-      <c r="I57" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="I57" s="13"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
@@ -5828,9 +5763,7 @@
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
-      <c r="L66" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="L66" s="13"/>
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -5901,9 +5834,7 @@
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
-      <c r="L67" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="L67" s="13"/>
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -5974,9 +5905,7 @@
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
-      <c r="L68" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="L68" s="13"/>
       <c r="M68" s="5"/>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
@@ -6047,9 +5976,7 @@
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
-      <c r="L69" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="L69" s="13"/>
       <c r="M69" s="5"/>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -6104,20 +6031,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="4">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
       <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
+      <c r="I70" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="J70" s="13"/>
       <c r="K70" s="13"/>
       <c r="L70" s="13"/>
@@ -6175,14 +6104,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="4">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
@@ -6246,14 +6175,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="4">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E72" s="13"/>
       <c r="F72" s="13"/>
@@ -6317,14 +6246,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="4">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
@@ -6388,14 +6317,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="4">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
@@ -6459,14 +6388,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="4">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
@@ -6530,14 +6459,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="4">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E76" s="13"/>
       <c r="F76" s="13"/>
@@ -6601,14 +6530,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="4">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
@@ -6672,14 +6601,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="4">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
@@ -6743,14 +6672,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="4">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
@@ -6814,14 +6743,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="4">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E80" s="13"/>
       <c r="F80" s="13"/>
@@ -6885,14 +6814,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="4">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E81" s="13"/>
       <c r="F81" s="13"/>
@@ -6956,14 +6885,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="4">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
@@ -7027,14 +6956,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="4">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E83" s="13"/>
       <c r="F83" s="13"/>
@@ -7098,14 +7027,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="4">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
@@ -7169,14 +7098,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="4">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E85" s="13"/>
       <c r="F85" s="13"/>
@@ -7240,14 +7169,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="4">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -7311,14 +7240,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="4">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" s="13"/>
       <c r="F87" s="13"/>
@@ -7382,14 +7311,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="4">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E88" s="13"/>
       <c r="F88" s="13"/>
@@ -7453,14 +7382,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="4">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>

</xml_diff>